<commit_message>
code updated to work with Cust_Leg_Name
</commit_message>
<xml_diff>
--- a/clientTestData/JMH.xlsx
+++ b/clientTestData/JMH.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulaxmira/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulaxmira/Documents/RallyMochaFramework/clientTestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F5858B-D2A1-C549-8716-E7DF5C4B32DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FF43F3-0CED-7B47-9B7C-CA6F7D361139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
     <t>PROD_JMH_AUM_AFF1a@mailinator.com</t>
   </si>
   <si>
-    <t>John Muir Health</t>
+    <t>Fluor Corporate</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>